<commit_message>
Updated BOM again (hopefully it is finished)
</commit_message>
<xml_diff>
--- a/Hardware/Science Actuation/Science_Actuation.xlsx
+++ b/Hardware/Science Actuation/Science_Actuation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Github\ScienceActuation_Hardware\Hardware\Science Actuation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurum\OneDrive\Documents\GitHub\ScienceActuation_Hardware\Hardware\Science Actuation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C2B061-2A4F-47EB-84B9-713472F3CED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89672FDA-BA30-421A-8821-16697C143C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Science_Actuation" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="181">
   <si>
     <t>Value</t>
   </si>
@@ -278,18 +276,6 @@
     <t>4700 Ω</t>
   </si>
   <si>
-    <t>560 Ω</t>
-  </si>
-  <si>
-    <t>2200 Ω</t>
-  </si>
-  <si>
-    <t>300 Ω</t>
-  </si>
-  <si>
-    <t>30 Ω</t>
-  </si>
-  <si>
     <t>Switch</t>
   </si>
   <si>
@@ -311,15 +297,6 @@
     <t>https://www.digikey.com/en/products/detail/vishay-dale/CRCW06034K70FKEA/1174744</t>
   </si>
   <si>
-    <t>RC0603JR-07300RL</t>
-  </si>
-  <si>
-    <t>311-300GRTR-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/yageo/RC0603JR-07300RL/726765</t>
-  </si>
-  <si>
     <t>RMCF0603FT100R</t>
   </si>
   <si>
@@ -329,15 +306,6 @@
     <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603FT100R/1761113</t>
   </si>
   <si>
-    <t>ERJ-3GEYJ222V</t>
-  </si>
-  <si>
-    <t>P2.2KGTR-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-3GEYJ222V/135862</t>
-  </si>
-  <si>
     <t>SD0603S040S0R2</t>
   </si>
   <si>
@@ -480,13 +448,139 @@
   </si>
   <si>
     <t>https://www.pjrc.com/store/ethernet_kit.html</t>
+  </si>
+  <si>
+    <t>ESK107M025AE3EA</t>
+  </si>
+  <si>
+    <t>399-6650-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/ESK107M025AE3EA/3083065</t>
+  </si>
+  <si>
+    <t>25YXG220MEFC6.3X11</t>
+  </si>
+  <si>
+    <t>1189-1233-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rubycon/25YXG220MEFC6-3X11/3134189</t>
+  </si>
+  <si>
+    <t>ECA-1EHG331</t>
+  </si>
+  <si>
+    <t>P5542-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ECA-1EHG331/245141</t>
+  </si>
+  <si>
+    <t>25ZLH470MEFC10X12.5</t>
+  </si>
+  <si>
+    <t>1189-1869-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rubycon/25ZLH470MEFC10X12-5/3563614</t>
+  </si>
+  <si>
+    <t>CL10B104KA8NNNC</t>
+  </si>
+  <si>
+    <t>1276-1006-2-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10B104KA8NNNC/3886664</t>
+  </si>
+  <si>
+    <t>CL10A106MA8NRNC</t>
+  </si>
+  <si>
+    <t>1276-1869-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10A106MA8NRNC/3887527</t>
+  </si>
+  <si>
+    <t>CL10B105MO8NNWC</t>
+  </si>
+  <si>
+    <t>1276-6524-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10B105MO8NNWC/1276-6524-1-ND/5961383</t>
+  </si>
+  <si>
+    <t>SN74LVC2G04</t>
+  </si>
+  <si>
+    <t>2-CH Inverter</t>
+  </si>
+  <si>
+    <t>SN74LVC2G04DBVR</t>
+  </si>
+  <si>
+    <t>296-13261-2-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74LVC2G04DBVR/484834</t>
+  </si>
+  <si>
+    <t>820 Ω</t>
+  </si>
+  <si>
+    <t>RMCF0603FT820R</t>
+  </si>
+  <si>
+    <t>RMCF0603FT820RTR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603FT820R/1714260</t>
+  </si>
+  <si>
+    <t>3000 Ω</t>
+  </si>
+  <si>
+    <t>RC0603FR-133KL</t>
+  </si>
+  <si>
+    <t>13-RC0603FR-133KLCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603FR-133KL/14008166</t>
+  </si>
+  <si>
+    <t>330 Ω</t>
+  </si>
+  <si>
+    <t>RC0603JR-07330RL</t>
+  </si>
+  <si>
+    <t>311-330GRTR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603JR-07330RL/726769</t>
+  </si>
+  <si>
+    <t>220 Ω</t>
+  </si>
+  <si>
+    <t>RMCF0603JT220R</t>
+  </si>
+  <si>
+    <t>RMCF0603JT220RTR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603JT220R/1758014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,6 +733,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -983,7 +1098,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -992,6 +1107,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1052,9 +1190,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1092,7 +1230,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1198,7 +1336,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1340,7 +1478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1350,24 +1488,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" customWidth="1"/>
-    <col min="2" max="2" width="58.54296875" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="58.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" customWidth="1"/>
-    <col min="11" max="11" width="59.1796875" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="59.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1402,7 +1540,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1415,16 +1553,30 @@
       <c r="D3" t="s">
         <v>54</v>
       </c>
+      <c r="E3" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4">
+        <v>0.26</v>
+      </c>
       <c r="J3" s="4">
         <f>(I3*H3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>2.6</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1437,16 +1589,30 @@
       <c r="D4" t="s">
         <v>54</v>
       </c>
+      <c r="E4" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4">
+        <v>0.1</v>
+      </c>
       <c r="J4" s="4">
-        <f t="shared" ref="J4:J34" si="0">(I4*H4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" ref="J4:J30" si="0">(I4*H4)</f>
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1459,16 +1625,30 @@
       <c r="D5" t="s">
         <v>54</v>
       </c>
+      <c r="E5" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="H5">
         <v>8</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4">
+        <v>0.1</v>
+      </c>
       <c r="J5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.8</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1481,16 +1661,30 @@
       <c r="D6" t="s">
         <v>54</v>
       </c>
+      <c r="E6" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4">
+        <v>0.24</v>
+      </c>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.24</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1503,16 +1697,30 @@
       <c r="D7" t="s">
         <v>54</v>
       </c>
+      <c r="E7" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4">
+        <v>0.3</v>
+      </c>
       <c r="J7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.3</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1525,16 +1733,30 @@
       <c r="D8" t="s">
         <v>54</v>
       </c>
+      <c r="E8" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4">
+        <v>0.49</v>
+      </c>
       <c r="J8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.49</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1547,16 +1769,30 @@
       <c r="D9" t="s">
         <v>54</v>
       </c>
+      <c r="E9" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4">
+        <v>0.53</v>
+      </c>
       <c r="J9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.53</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1567,16 +1803,16 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G10" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H10">
         <v>10</v>
@@ -1589,10 +1825,10 @@
         <v>9.2000000000000011</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1600,7 +1836,7 @@
         <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D11" t="s">
         <v>58</v>
@@ -1609,10 +1845,10 @@
         <v>705430001</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H11">
         <v>6</v>
@@ -1625,10 +1861,10 @@
         <v>6.18</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1636,19 +1872,19 @@
         <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
         <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H12">
         <v>8</v>
@@ -1661,10 +1897,10 @@
         <v>3.04</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1678,13 +1914,13 @@
         <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1697,10 +1933,10 @@
         <v>0.34</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1714,13 +1950,13 @@
         <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F14" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -1733,14 +1969,14 @@
         <v>0.78</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1751,16 +1987,16 @@
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F16" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="G16" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1773,10 +2009,10 @@
         <v>3.9</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1784,19 +2020,19 @@
         <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="E17" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F17" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="G17" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="H17">
         <v>16</v>
@@ -1809,10 +2045,10 @@
         <v>14.4</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1829,10 +2065,10 @@
         <v>705430003</v>
       </c>
       <c r="F18" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H18">
         <v>4</v>
@@ -1845,10 +2081,10 @@
         <v>4.84</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1862,13 +2098,13 @@
         <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G19" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H19">
         <v>16</v>
@@ -1881,10 +2117,10 @@
         <v>1.6</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1898,13 +2134,13 @@
         <v>56</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H20">
         <v>6</v>
@@ -1917,10 +2153,10 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1928,21 +2164,35 @@
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="D21" t="s">
         <v>56</v>
       </c>
+      <c r="E21" t="s">
+        <v>166</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G21" t="s">
+        <v>86</v>
+      </c>
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="I21" s="4">
+        <v>0.1</v>
+      </c>
       <c r="J21" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.1</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1950,19 +2200,19 @@
         <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>169</v>
       </c>
       <c r="D22" t="s">
         <v>56</v>
       </c>
-      <c r="E22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" t="s">
-        <v>99</v>
+      <c r="E22" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>171</v>
       </c>
       <c r="G22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -1975,10 +2225,10 @@
         <v>0.1</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1986,19 +2236,19 @@
         <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
       <c r="D23" t="s">
         <v>56</v>
       </c>
-      <c r="E23" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" t="s">
-        <v>93</v>
+      <c r="E23" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="G23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2011,10 +2261,10 @@
         <v>0.1</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -2022,21 +2272,35 @@
         <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="D24" t="s">
         <v>56</v>
       </c>
+      <c r="E24" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="H24">
         <v>1</v>
       </c>
-      <c r="I24" s="4"/>
+      <c r="I24" s="4">
+        <v>0.1</v>
+      </c>
       <c r="J24" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.1</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2053,10 +2317,10 @@
         <v>705430002</v>
       </c>
       <c r="F25" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="G25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H25">
         <v>2</v>
@@ -2069,10 +2333,10 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2086,13 +2350,13 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F26" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H26">
         <v>6</v>
@@ -2105,10 +2369,10 @@
         <v>1.26</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2119,16 +2383,16 @@
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="F27" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="G27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -2141,10 +2405,10 @@
         <v>0.61</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2155,16 +2419,16 @@
         <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G28" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2177,10 +2441,10 @@
         <v>35.5</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2188,19 +2452,19 @@
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E29" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F29" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="G29" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -2213,26 +2477,46 @@
         <v>3.09</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>76</v>
       </c>
+      <c r="C30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D30" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F30" t="s">
+        <v>163</v>
+      </c>
+      <c r="G30" t="s">
+        <v>86</v>
+      </c>
       <c r="H30">
         <v>4</v>
       </c>
-      <c r="I30" s="4"/>
+      <c r="I30" s="4">
+        <v>0.46</v>
+      </c>
       <c r="J30" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.84</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2240,19 +2524,19 @@
         <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D31" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E31" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F31" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="G31" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H31">
         <v>8</v>
@@ -2265,10 +2549,10 @@
         <v>10.72</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -2277,22 +2561,32 @@
   <phoneticPr fontId="20" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K20" r:id="rId1" xr:uid="{A10CE770-D096-4F94-A39F-B1BE83C6315F}"/>
-    <hyperlink ref="K23" r:id="rId2" xr:uid="{A0F907DA-7174-4D3E-A83D-B6489F2FFCCB}"/>
-    <hyperlink ref="K19" r:id="rId3" xr:uid="{9D98BD1B-7510-4E50-9F6A-6DE0EC182833}"/>
-    <hyperlink ref="K12" r:id="rId4" xr:uid="{F05BE3B1-2E61-46A6-AA27-0D99927327C3}"/>
-    <hyperlink ref="K13" r:id="rId5" xr:uid="{7EE06DC6-489A-4140-8177-EA27ED70AAA1}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{55282F9D-AF8C-4143-890D-0128AE9B35F7}"/>
-    <hyperlink ref="K11" r:id="rId7" xr:uid="{CC275032-3589-4A46-A054-4544EAB9A913}"/>
-    <hyperlink ref="K26" r:id="rId8" xr:uid="{E066871D-3BB9-4082-B03E-1988AF9816B3}"/>
-    <hyperlink ref="K27" r:id="rId9" xr:uid="{B57761FF-A121-4623-A887-3E283F45AC04}"/>
-    <hyperlink ref="K10" r:id="rId10" xr:uid="{AD8E5EA3-1EC3-4D58-AEB9-8338D73BB957}"/>
-    <hyperlink ref="K29" r:id="rId11" xr:uid="{43DBC8D2-13F8-4DA3-BD36-1753F033E5DB}"/>
-    <hyperlink ref="K28" r:id="rId12" xr:uid="{6A769AD9-E1C0-4CE6-85F6-C100EBD65701}"/>
-    <hyperlink ref="K31" r:id="rId13" xr:uid="{A66B12C2-0F8A-463A-B120-E0627AC8DA76}"/>
-    <hyperlink ref="K25" r:id="rId14" xr:uid="{F743A4FC-C48A-407E-B3FF-A45A23B1D8D3}"/>
-    <hyperlink ref="K18" r:id="rId15" xr:uid="{7AAC0AA3-FA79-4CB3-AFC8-B9DDF2E9BB3F}"/>
-    <hyperlink ref="K17" r:id="rId16" xr:uid="{243F4D97-F42F-4AC7-97DC-558E3E441FD0}"/>
-    <hyperlink ref="K16" r:id="rId17" xr:uid="{DF128B8D-ABCD-410E-8F19-8819F7C90C68}"/>
+    <hyperlink ref="K19" r:id="rId2" xr:uid="{9D98BD1B-7510-4E50-9F6A-6DE0EC182833}"/>
+    <hyperlink ref="K12" r:id="rId3" xr:uid="{F05BE3B1-2E61-46A6-AA27-0D99927327C3}"/>
+    <hyperlink ref="K13" r:id="rId4" xr:uid="{7EE06DC6-489A-4140-8177-EA27ED70AAA1}"/>
+    <hyperlink ref="K14" r:id="rId5" xr:uid="{55282F9D-AF8C-4143-890D-0128AE9B35F7}"/>
+    <hyperlink ref="K11" r:id="rId6" xr:uid="{CC275032-3589-4A46-A054-4544EAB9A913}"/>
+    <hyperlink ref="K26" r:id="rId7" xr:uid="{E066871D-3BB9-4082-B03E-1988AF9816B3}"/>
+    <hyperlink ref="K27" r:id="rId8" xr:uid="{B57761FF-A121-4623-A887-3E283F45AC04}"/>
+    <hyperlink ref="K10" r:id="rId9" xr:uid="{AD8E5EA3-1EC3-4D58-AEB9-8338D73BB957}"/>
+    <hyperlink ref="K29" r:id="rId10" xr:uid="{43DBC8D2-13F8-4DA3-BD36-1753F033E5DB}"/>
+    <hyperlink ref="K28" r:id="rId11" xr:uid="{6A769AD9-E1C0-4CE6-85F6-C100EBD65701}"/>
+    <hyperlink ref="K31" r:id="rId12" xr:uid="{A66B12C2-0F8A-463A-B120-E0627AC8DA76}"/>
+    <hyperlink ref="K25" r:id="rId13" xr:uid="{F743A4FC-C48A-407E-B3FF-A45A23B1D8D3}"/>
+    <hyperlink ref="K18" r:id="rId14" xr:uid="{7AAC0AA3-FA79-4CB3-AFC8-B9DDF2E9BB3F}"/>
+    <hyperlink ref="K17" r:id="rId15" xr:uid="{243F4D97-F42F-4AC7-97DC-558E3E441FD0}"/>
+    <hyperlink ref="K16" r:id="rId16" xr:uid="{DF128B8D-ABCD-410E-8F19-8819F7C90C68}"/>
+    <hyperlink ref="K6" r:id="rId17" xr:uid="{6EFE3F0B-49EE-4DA2-BD37-8A432B3CDC4C}"/>
+    <hyperlink ref="K8" r:id="rId18" xr:uid="{9791EEF3-A830-48AF-B69E-C06277180C86}"/>
+    <hyperlink ref="K7" r:id="rId19" xr:uid="{522596A7-B553-4B39-84E2-72EFA0B0063F}"/>
+    <hyperlink ref="K4" r:id="rId20" xr:uid="{47C9BFF1-8C1F-4066-AA39-D3A385A4DC3F}"/>
+    <hyperlink ref="K3" r:id="rId21" xr:uid="{85E5DDB3-C6F6-490E-B841-9E69FDAE033C}"/>
+    <hyperlink ref="K5" r:id="rId22" xr:uid="{167EDB5E-DB20-4A4C-BE4D-37B574DBC43F}"/>
+    <hyperlink ref="K9" r:id="rId23" xr:uid="{3273759A-D60E-40B2-A578-8A78F81F2C36}"/>
+    <hyperlink ref="K30" r:id="rId24" xr:uid="{7CCCF161-C7FD-482A-862E-74A5B5427D90}"/>
+    <hyperlink ref="K21" r:id="rId25" xr:uid="{D34A7772-81F5-4B26-9628-A661E9E90C4E}"/>
+    <hyperlink ref="K22" r:id="rId26" xr:uid="{5323659F-B3BE-4137-A698-28A26A0B4E49}"/>
+    <hyperlink ref="K24" r:id="rId27" xr:uid="{198FBAC9-FA4A-4884-9156-D31BAE513199}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>